<commit_message>
Update HW: Access COntrol
</commit_message>
<xml_diff>
--- a/HW/Source/BluetoothGateway/Project Outputs for BluetoothGateway/BOM_BluetoothGateway.xlsx
+++ b/HW/Source/BluetoothGateway/Project Outputs for BluetoothGateway/BOM_BluetoothGateway.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BLUETOOTH_TRACKING\HW\Source\BluetoothGateway\Project Outputs for BluetoothGateway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0CCFAD-A868-41D0-83A7-E348D7531F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC15D90-07AC-4654-84FD-319A1204F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F049304F-4970-4728-9571-4B65C25DB4FD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{F049304F-4970-4728-9571-4B65C25DB4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_BluetoothGateway" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>tme</t>
   </si>
   <si>
-    <t>http://www.tme.vn/Product.aspx?id=1165#page=pro_info</t>
-  </si>
-  <si>
     <t>C24, C25</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>Buck Switching Regulator IC Positive Adjustable 0.8V 1 Output 3A 8-SOIC _0.154, 3.90mm Width_ Exposed Pad</t>
   </si>
   <si>
-    <t>http://www.tme.vn/Product.aspx?id=2070#page=pro_info</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -493,13 +487,19 @@
   </si>
   <si>
     <t>https://www.thegioiic.com/thach-anh-25mhz-3225-4-chan-smd</t>
+  </si>
+  <si>
+    <t>http://tme.vn/Product.aspx?id=1165#page=pro_info</t>
+  </si>
+  <si>
+    <t>http://tme.vn/Product.aspx?id=2070#page=pro_info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,16 +507,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,18 +518,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,10 +555,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,19 +895,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29E34DE-ADC5-4CD3-90F0-4149558439F8}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="116.7109375" customWidth="1"/>
+    <col min="1" max="2" width="19.73046875" customWidth="1"/>
+    <col min="3" max="3" width="67.73046875" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" customWidth="1"/>
+    <col min="5" max="5" width="116.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -944,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -957,7 +937,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -974,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -991,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1008,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1005,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1059,7 +1039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1076,7 +1056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1093,7 +1073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -1106,166 +1086,166 @@
       <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
@@ -1280,332 +1260,332 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="7" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="B30" s="1">
         <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="8" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="B39" s="1">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1617,12 +1597,12 @@
         <v>9</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" s="2" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1634,46 +1614,46 @@
         <v>9</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1684,9 +1664,9 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -1697,9 +1677,9 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -1710,9 +1690,9 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -1723,9 +1703,9 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -1736,9 +1716,9 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -1749,9 +1729,9 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -1762,123 +1742,123 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B57" s="1">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B58" s="1">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>